<commit_message>
changed code for ppcb and case
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/wireless_UA_fencing_scoring_box/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F558B1-F233-DF48-8C97-62ED2A2AD6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CF8F7-20AB-8D4E-B07C-85CCFD280F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{E9CEC752-5B2B-0E4B-B3C6-22486103B0E7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16260" xr2:uid="{E9CEC752-5B2B-0E4B-B3C6-22486103B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Wireless Box BOM</t>
   </si>
@@ -44,15 +44,9 @@
     <t>Seeed XIAO (x3)</t>
   </si>
   <si>
-    <t>NRF24 (x6)</t>
-  </si>
-  <si>
     <t>Buzzer (x10)</t>
   </si>
   <si>
-    <t>Seeed Shield (x3)</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -62,15 +56,9 @@
     <t>Buzzer (x1)</t>
   </si>
   <si>
-    <t>NRF24 (x3)</t>
-  </si>
-  <si>
     <t>Banana Jacks (x6)</t>
   </si>
   <si>
-    <t>LiPo Batteries (x3)</t>
-  </si>
-  <si>
     <t>Total Order</t>
   </si>
   <si>
@@ -83,10 +71,37 @@
     <t>Per Box</t>
   </si>
   <si>
-    <t>LiPo Batteries (x4)</t>
-  </si>
-  <si>
     <t>Banana Jacks (x20)</t>
+  </si>
+  <si>
+    <t>NRF24 SMD (x10)</t>
+  </si>
+  <si>
+    <t>AMS1117</t>
+  </si>
+  <si>
+    <t>AMS1117 (x10)</t>
+  </si>
+  <si>
+    <t>Power Banks (x3)</t>
+  </si>
+  <si>
+    <t>LEDs (x450)</t>
+  </si>
+  <si>
+    <t>1k ohm (x100)</t>
+  </si>
+  <si>
+    <t>NRF24 SMD (x3)</t>
+  </si>
+  <si>
+    <t>Power Banks</t>
+  </si>
+  <si>
+    <t>LEDs (x4)</t>
+  </si>
+  <si>
+    <t>Resistors (x6)</t>
   </si>
 </sst>
 </file>
@@ -110,10 +125,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -122,12 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BE97A9-762F-D441-9D12-CBDDC71003E9}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,22 +487,22 @@
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -483,41 +510,40 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>5.4*3</f>
-        <v>16.200000000000003</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3">
         <f>B3</f>
-        <v>16.200000000000003</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>12.39</v>
+        <v>10.88</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E4">
-        <f>B4/2</f>
-        <v>6.1950000000000003</v>
+        <f>(B4/10)*3</f>
+        <v>3.2640000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <f>7/10</f>
@@ -526,13 +552,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <f>(B6/20)*6</f>
@@ -541,18 +567,17 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <f>4.5*3</f>
-        <v>13.5</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <f>B7</f>
-        <v>13.5</v>
+        <f>B7/10*3</f>
+        <v>2.4000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -560,35 +585,64 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E8">
-        <f>(B8/4)*3</f>
-        <v>7.5</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f>B9/450*4</f>
+        <v>0.11555555555555555</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <f>SUM(B3:B8)</f>
-        <v>70.09</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E10">
-        <f>SUM(E3:E8)</f>
-        <v>47.395000000000003</v>
+        <f>B10/100*6</f>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B3:B10)</f>
+        <v>105.88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f>SUM(E3:E8)</f>
+        <v>60.663999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>